<commit_message>
increased coverage for xlsx parser
</commit_message>
<xml_diff>
--- a/mtd/tests/test_data/xlsx/data.xlsx
+++ b/mtd/tests/test_data/xlsx/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>word</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>ap_red_def.mp3</t>
-  </si>
-  <si>
-    <t>ar_red_def.mp3</t>
   </si>
   <si>
     <t>Har du røde øjne?</t>
@@ -197,9 +194,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -213,18 +214,35 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -357,6 +375,8 @@
       <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -398,75 +418,73 @@
       <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AE2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AI2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>